<commit_message>
feat: add the import function and fix some bugs
</commit_message>
<xml_diff>
--- a/ledger.xlsx
+++ b/ledger.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="2024-12" sheetId="1" r:id="rId1"/>
+    <sheet name="2023-01" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="12">
   <si>
     <t>月</t>
   </si>
@@ -25,6 +26,12 @@
     <t>摘要</t>
   </si>
   <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <t>账户</t>
+  </si>
+  <si>
     <t>收入</t>
   </si>
   <si>
@@ -35,6 +42,15 @@
   </si>
   <si>
     <t>dinner</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>alipay</t>
+  </si>
+  <si>
+    <t>wechat</t>
   </si>
 </sst>
 </file>
@@ -366,13 +382,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,8 +407,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>12</v>
       </c>
@@ -400,16 +422,22 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>532.87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>1029.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>12</v>
       </c>
@@ -417,16 +445,22 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>532.87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>12</v>
       </c>
@@ -434,16 +468,22 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>532.87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>1009.5999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>12</v>
       </c>
@@ -451,16 +491,22 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>532.87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>1019.5999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>12</v>
       </c>
@@ -468,13 +514,196 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>20.4</v>
+      </c>
+      <c r="H7">
+        <v>1049.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>1039.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>522.87</v>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>23</v>
+      </c>
+      <c r="H2">
+        <v>986.5999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>963.5999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>23</v>
+      </c>
+      <c r="H4">
+        <v>940.5999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>917.5999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fix the export excel format
</commit_message>
<xml_diff>
--- a/ledger.xlsx
+++ b/ledger.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="2024-12" sheetId="1" r:id="rId1"/>
-    <sheet name="2023-01" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="24">
   <si>
     <t>月</t>
   </si>
@@ -50,15 +49,62 @@
     <t>alipay</t>
   </si>
   <si>
+    <t>bankofchina</t>
+  </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
     <t>wechat</t>
+  </si>
+  <si>
+    <t>breakfast</t>
+  </si>
+  <si>
+    <t>kfc</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>study</t>
+  </si>
+  <si>
+    <t>打印</t>
+  </si>
+  <si>
+    <t>校园卡充值</t>
+  </si>
+  <si>
+    <t>life</t>
+  </si>
+  <si>
+    <t>购物</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>rest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00"/>
+  </numFmts>
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -86,8 +132,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,35 +432,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -430,11 +480,11 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>1029.6</v>
+      <c r="G2" s="2">
+        <v>10</v>
+      </c>
+      <c r="H2" s="2">
+        <v>532.87</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -453,11 +503,11 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>1100</v>
+      <c r="G3" s="2">
+        <v>10</v>
+      </c>
+      <c r="H3" s="2">
+        <v>532.87</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -476,11 +526,11 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>1009.5999999999999</v>
+      <c r="G4" s="2">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2">
+        <v>532.87</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -497,13 +547,13 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>1019.5999999999999</v>
+        <v>11</v>
+      </c>
+      <c r="G5" s="2">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2">
+        <v>532.87</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -522,11 +572,11 @@
       <c r="E6" t="s">
         <v>11</v>
       </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-      <c r="H6">
-        <v>1070</v>
+      <c r="G6" s="2">
+        <v>10</v>
+      </c>
+      <c r="H6" s="2">
+        <v>522.87</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -534,7 +584,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -543,13 +593,13 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7">
-        <v>20.4</v>
-      </c>
-      <c r="H7">
-        <v>1049.6</v>
+        <v>10</v>
+      </c>
+      <c r="G7" s="2">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2">
+        <v>470.87</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -557,7 +607,7 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -568,142 +618,402 @@
       <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>1039.6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="G8" s="2">
+        <v>20</v>
+      </c>
+      <c r="H8" s="2">
+        <v>450.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2">
+        <v>540.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="2">
+        <v>30</v>
+      </c>
+      <c r="H10" s="2">
+        <v>570.87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2">
+        <v>560.87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2">
+        <v>20</v>
+      </c>
+      <c r="H12" s="2">
+        <v>540.87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2">
+        <v>510.87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="2">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2">
+        <v>520.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2">
+        <v>12</v>
+      </c>
+      <c r="H15" s="2">
+        <v>510.87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2">
+        <v>20</v>
+      </c>
+      <c r="H16" s="2">
+        <v>490.87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2">
+        <v>40</v>
+      </c>
+      <c r="H17" s="2">
+        <v>410.87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
+      <c r="H18" s="2">
+        <v>410.87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="H19" s="2">
+        <v>410.42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="2">
+        <v>130</v>
+      </c>
+      <c r="H20" s="2">
+        <v>280.42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2">
+        <v>85.7</v>
+      </c>
+      <c r="H21" s="2">
+        <v>194.72000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="2">
+        <v>2000</v>
+      </c>
+      <c r="H22" s="2">
+        <v>-1805.28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H23" s="2">
+        <v>-2805.2799999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2">
+        <v>800</v>
+      </c>
+      <c r="H24" s="2">
+        <v>-3605.2799999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
         <v>23</v>
       </c>
-      <c r="H2">
-        <v>986.5999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>23</v>
-      </c>
-      <c r="H3">
-        <v>963.5999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>23</v>
-      </c>
-      <c r="H4">
-        <v>940.5999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>23</v>
-      </c>
-      <c r="H5">
-        <v>917.5999999999999</v>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="2">
+        <v>600</v>
+      </c>
+      <c r="H25" s="2">
+        <v>-4205.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>